<commit_message>
Finished Testing of IterationRecord and Export Functionality
</commit_message>
<xml_diff>
--- a/FunctionalityTests/IterationRecordTests.xlsx
+++ b/FunctionalityTests/IterationRecordTests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="1300" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="43200" yWindow="2560" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,12 +86,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -106,13 +112,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,8 +399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,6 +448,7 @@
       <c r="E2" t="b">
         <v>0</v>
       </c>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -458,6 +466,7 @@
       <c r="E3" t="b">
         <v>0</v>
       </c>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -475,6 +484,7 @@
       <c r="E4" t="b">
         <v>0</v>
       </c>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -492,6 +502,7 @@
       <c r="E5" t="b">
         <v>1</v>
       </c>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -509,6 +520,7 @@
       <c r="E6" t="b">
         <v>1</v>
       </c>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -526,6 +538,7 @@
       <c r="E7" t="b">
         <v>1</v>
       </c>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
@@ -543,6 +556,7 @@
       <c r="E8" t="b">
         <v>0</v>
       </c>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -560,6 +574,7 @@
       <c r="E9" t="b">
         <v>0</v>
       </c>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -577,6 +592,7 @@
       <c r="E10" t="b">
         <v>0</v>
       </c>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
@@ -594,6 +610,7 @@
       <c r="E11" t="b">
         <v>1</v>
       </c>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -611,6 +628,7 @@
       <c r="E12" t="b">
         <v>1</v>
       </c>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -628,6 +646,7 @@
       <c r="E13" t="b">
         <v>1</v>
       </c>
+      <c r="F13" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -645,6 +664,7 @@
       <c r="E15" t="b">
         <v>0</v>
       </c>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -662,8 +682,9 @@
       <c r="E16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
@@ -679,8 +700,9 @@
       <c r="E17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
@@ -696,8 +718,9 @@
       <c r="E18" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>9</v>
       </c>
@@ -713,8 +736,9 @@
       <c r="E19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
@@ -730,8 +754,9 @@
       <c r="E20" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
@@ -747,8 +772,9 @@
       <c r="E21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
@@ -764,8 +790,9 @@
       <c r="E22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -781,8 +808,9 @@
       <c r="E23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
@@ -798,8 +826,9 @@
       <c r="E24" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>9</v>
       </c>
@@ -815,8 +844,9 @@
       <c r="E25" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>9</v>
       </c>
@@ -832,8 +862,9 @@
       <c r="E26" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="4"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>10</v>
       </c>
@@ -849,8 +880,9 @@
       <c r="E28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>10</v>
       </c>
@@ -866,8 +898,9 @@
       <c r="E29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>10</v>
       </c>
@@ -883,8 +916,9 @@
       <c r="E30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>10</v>
       </c>
@@ -900,8 +934,9 @@
       <c r="E31" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>10</v>
       </c>
@@ -917,8 +952,9 @@
       <c r="E32" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>10</v>
       </c>
@@ -934,8 +970,9 @@
       <c r="E33" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>10</v>
       </c>
@@ -951,8 +988,9 @@
       <c r="E34" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>10</v>
       </c>
@@ -968,8 +1006,9 @@
       <c r="E35" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>10</v>
       </c>
@@ -985,8 +1024,9 @@
       <c r="E36" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>10</v>
       </c>
@@ -1002,8 +1042,9 @@
       <c r="E37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>10</v>
       </c>
@@ -1019,8 +1060,9 @@
       <c r="E38" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>10</v>
       </c>
@@ -1036,6 +1078,7 @@
       <c r="E39" t="b">
         <v>1</v>
       </c>
+      <c r="F39" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>